<commit_message>
Increased time period for a work item.
</commit_message>
<xml_diff>
--- a/Documentation/Sprint Plans.xlsx
+++ b/Documentation/Sprint Plans.xlsx
@@ -462,9 +462,156 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <left style="thin">
           <color rgb="FF000000"/>
-        </bottom>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -487,6 +634,13 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -610,35 +764,35 @@
     <dxf>
       <border outline="0">
         <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
+          <color indexed="64"/>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
         <left style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -650,160 +804,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -820,22 +820,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B11:G26" totalsRowShown="0" headerRowDxfId="22" dataDxfId="23" headerRowBorderDxfId="31" tableBorderDxfId="32" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B11:G26" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="B11:G26"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID:" dataDxfId="29"/>
-    <tableColumn id="2" name="Task:" dataDxfId="28"/>
-    <tableColumn id="3" name="Assigned To:" dataDxfId="27"/>
-    <tableColumn id="4" name="Effort Points:" dataDxfId="26"/>
-    <tableColumn id="5" name="Estimated Hours:" dataDxfId="25"/>
-    <tableColumn id="6" name="Status:" dataDxfId="24"/>
+    <tableColumn id="1" name="ID:" dataDxfId="27"/>
+    <tableColumn id="2" name="Task:" dataDxfId="26"/>
+    <tableColumn id="3" name="Assigned To:" dataDxfId="25"/>
+    <tableColumn id="4" name="Effort Points:" dataDxfId="24"/>
+    <tableColumn id="5" name="Estimated Hours:" dataDxfId="23"/>
+    <tableColumn id="6" name="Status:" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:G26" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B11:G26" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B11:G26"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID:" dataDxfId="16"/>
@@ -850,7 +850,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B11:G26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B11:G26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B11:G26"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID:" dataDxfId="5"/>
@@ -1130,7 +1130,7 @@
   <dimension ref="B2:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1290,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>10</v>

</xml_diff>